<commit_message>
[Matteo,Sandra,Yusuf] [Task: Write DOCUMENTATION.md] Wrote chapter on prompt engineering
</commit_message>
<xml_diff>
--- a/project/evaluation/llm_evaluation/prompt_engineering/results/Interpretation of the results of Promt Engineering.xlsx
+++ b/project/evaluation/llm_evaluation/prompt_engineering/results/Interpretation of the results of Promt Engineering.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteom/shared-folder/nlpt_group/project/evaluation/llm_evaluation/results/prompt_engineering/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteom/shared-folder/nlpt_group/project/evaluation/llm_evaluation/prompt_engineering/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25500D12-F1C6-724B-B6FA-C47D87C4BD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD58754-E70D-0E4A-829A-B1F8CDCCE8B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" xr2:uid="{F45BEFED-20B5-344B-A934-62A103900DF0}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{F45BEFED-20B5-344B-A934-62A103900DF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -851,7 +851,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -867,15 +867,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -909,14 +900,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
@@ -924,39 +912,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
@@ -967,50 +922,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1024,12 +940,6 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1037,8 +947,89 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1386,8 +1377,8 @@
   <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6:P6"/>
+      <pane ySplit="2" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C54" sqref="C54:L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1406,983 +1397,983 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="102"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="97"/>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="5"/>
-      <c r="D2" s="9">
+      <c r="D2" s="6">
         <v>0</v>
       </c>
-      <c r="E2" s="10">
-        <v>1</v>
-      </c>
-      <c r="F2" s="10">
+      <c r="E2" s="7">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7">
         <v>2</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="7">
         <v>3</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="7">
         <v>4</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="44">
-        <v>1</v>
-      </c>
-      <c r="C3" s="55" t="s">
+      <c r="A3" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="91">
+        <v>1</v>
+      </c>
+      <c r="C3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="23">
-        <v>1</v>
-      </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24">
-        <v>1</v>
-      </c>
-      <c r="J3" s="25"/>
+      <c r="D3" s="20">
+        <v>1</v>
+      </c>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21">
+        <v>1</v>
+      </c>
+      <c r="J3" s="22"/>
     </row>
     <row r="4" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="56" t="s">
+      <c r="A4" s="77"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="27">
-        <v>1</v>
-      </c>
-      <c r="F4" s="27">
-        <v>1</v>
-      </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="28">
-        <v>1</v>
-      </c>
-      <c r="L4" s="80" t="s">
+      <c r="D4" s="23"/>
+      <c r="E4" s="24">
+        <v>1</v>
+      </c>
+      <c r="F4" s="24">
+        <v>1</v>
+      </c>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="25">
+        <v>1</v>
+      </c>
+      <c r="L4" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="82"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="68"/>
+      <c r="P4" s="69"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="57" t="s">
+      <c r="A5" s="77"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="26">
-        <v>1</v>
-      </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27">
-        <v>1</v>
-      </c>
-      <c r="J5" s="28"/>
-      <c r="L5" s="77" t="s">
+      <c r="D5" s="23">
+        <v>1</v>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24">
+        <v>1</v>
+      </c>
+      <c r="J5" s="25"/>
+      <c r="L5" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="78"/>
-      <c r="P5" s="79"/>
+      <c r="M5" s="86"/>
+      <c r="N5" s="86"/>
+      <c r="O5" s="86"/>
+      <c r="P5" s="87"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="47">
+      <c r="A6" s="77"/>
+      <c r="B6" s="88">
         <v>2</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="28"/>
-      <c r="L6" s="72" t="s">
+      <c r="D6" s="23"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="25"/>
+      <c r="L6" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="M6" s="71"/>
-      <c r="N6" s="71"/>
-      <c r="O6" s="71"/>
-      <c r="P6" s="73"/>
+      <c r="M6" s="83"/>
+      <c r="N6" s="83"/>
+      <c r="O6" s="83"/>
+      <c r="P6" s="84"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="56" t="s">
+      <c r="A7" s="77"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="29">
-        <v>1</v>
-      </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="30">
-        <v>1</v>
-      </c>
-      <c r="J7" s="28">
-        <v>1</v>
-      </c>
-      <c r="L7" s="72" t="s">
+      <c r="D7" s="23">
+        <v>1</v>
+      </c>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24">
+        <v>1</v>
+      </c>
+      <c r="J7" s="25">
+        <v>1</v>
+      </c>
+      <c r="L7" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="71"/>
-      <c r="N7" s="71"/>
-      <c r="O7" s="71"/>
-      <c r="P7" s="73"/>
+      <c r="M7" s="83"/>
+      <c r="N7" s="83"/>
+      <c r="O7" s="83"/>
+      <c r="P7" s="84"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="57" t="s">
+      <c r="A8" s="77"/>
+      <c r="B8" s="92"/>
+      <c r="C8" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27">
-        <v>1</v>
-      </c>
-      <c r="J8" s="28"/>
-      <c r="L8" s="72" t="s">
+      <c r="D8" s="23"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24">
+        <v>1</v>
+      </c>
+      <c r="J8" s="25"/>
+      <c r="L8" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="71"/>
-      <c r="N8" s="71"/>
-      <c r="O8" s="71"/>
-      <c r="P8" s="73"/>
+      <c r="M8" s="83"/>
+      <c r="N8" s="83"/>
+      <c r="O8" s="83"/>
+      <c r="P8" s="84"/>
     </row>
     <row r="9" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="47">
+      <c r="A9" s="77"/>
+      <c r="B9" s="88">
         <v>3</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27">
-        <v>1</v>
-      </c>
-      <c r="J9" s="28">
-        <v>1</v>
-      </c>
-      <c r="L9" s="74" t="s">
+      <c r="D9" s="23"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24">
+        <v>1</v>
+      </c>
+      <c r="J9" s="25">
+        <v>1</v>
+      </c>
+      <c r="L9" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="75"/>
-      <c r="P9" s="76"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="80"/>
+      <c r="O9" s="80"/>
+      <c r="P9" s="81"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="56" t="s">
+      <c r="A10" s="77"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="26">
-        <v>1</v>
-      </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27">
-        <v>1</v>
-      </c>
-      <c r="G10" s="27">
-        <v>1</v>
-      </c>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="28">
+      <c r="D10" s="23">
+        <v>1</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24">
+        <v>1</v>
+      </c>
+      <c r="G10" s="24">
+        <v>1</v>
+      </c>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="57" t="s">
+      <c r="A11" s="77"/>
+      <c r="B11" s="92"/>
+      <c r="C11" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27">
-        <v>1</v>
-      </c>
-      <c r="J11" s="28"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24">
+        <v>1</v>
+      </c>
+      <c r="J11" s="25"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="47">
+      <c r="A12" s="77"/>
+      <c r="B12" s="88">
         <v>4</v>
       </c>
-      <c r="C12" s="58" t="s">
+      <c r="C12" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27">
-        <v>1</v>
-      </c>
-      <c r="J12" s="28"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24">
+        <v>1</v>
+      </c>
+      <c r="J12" s="25"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="45"/>
-      <c r="C13" s="56" t="s">
+      <c r="A13" s="77"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="26">
-        <v>1</v>
-      </c>
-      <c r="E13" s="27">
-        <v>1</v>
-      </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="28">
+      <c r="D13" s="23">
+        <v>1</v>
+      </c>
+      <c r="E13" s="24">
+        <v>1</v>
+      </c>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="57" t="s">
+      <c r="A14" s="77"/>
+      <c r="B14" s="92"/>
+      <c r="C14" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27">
-        <v>1</v>
-      </c>
-      <c r="J14" s="28"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24">
+        <v>1</v>
+      </c>
+      <c r="J14" s="25"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="47">
+      <c r="A15" s="77"/>
+      <c r="B15" s="88">
         <v>5</v>
       </c>
-      <c r="C15" s="58" t="s">
+      <c r="C15" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27">
-        <v>1</v>
-      </c>
-      <c r="J15" s="28"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24">
+        <v>1</v>
+      </c>
+      <c r="J15" s="25"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
-      <c r="B16" s="45"/>
-      <c r="C16" s="56" t="s">
+      <c r="A16" s="77"/>
+      <c r="B16" s="89"/>
+      <c r="C16" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="26">
-        <v>1</v>
-      </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="28">
+      <c r="D16" s="23">
+        <v>1</v>
+      </c>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="57" t="s">
+      <c r="A17" s="77"/>
+      <c r="B17" s="92"/>
+      <c r="C17" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27">
-        <v>1</v>
-      </c>
-      <c r="J17" s="28">
+      <c r="D17" s="23"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24">
+        <v>1</v>
+      </c>
+      <c r="J17" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
-      <c r="B18" s="47">
+      <c r="A18" s="77"/>
+      <c r="B18" s="88">
         <v>6</v>
       </c>
-      <c r="C18" s="58" t="s">
+      <c r="C18" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="28"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="25"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="B19" s="45"/>
-      <c r="C19" s="56" t="s">
+      <c r="A19" s="77"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="26">
-        <v>1</v>
-      </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="30">
-        <v>1</v>
-      </c>
-      <c r="J19" s="28"/>
+      <c r="D19" s="23">
+        <v>1</v>
+      </c>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24">
+        <v>1</v>
+      </c>
+      <c r="J19" s="25"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="57" t="s">
+      <c r="A20" s="77"/>
+      <c r="B20" s="92"/>
+      <c r="C20" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27">
-        <v>1</v>
-      </c>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27">
-        <v>1</v>
-      </c>
-      <c r="J20" s="28"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24">
+        <v>1</v>
+      </c>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24">
+        <v>1</v>
+      </c>
+      <c r="J20" s="25"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="B21" s="47">
+      <c r="A21" s="77"/>
+      <c r="B21" s="88">
         <v>7</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="C21" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27">
-        <v>1</v>
-      </c>
-      <c r="J21" s="28"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24">
+        <v>1</v>
+      </c>
+      <c r="J21" s="25"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="56" t="s">
+      <c r="A22" s="77"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="27">
-        <v>1</v>
-      </c>
-      <c r="F22" s="27">
-        <v>1</v>
-      </c>
-      <c r="G22" s="27">
-        <v>1</v>
-      </c>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="28"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="24">
+        <v>1</v>
+      </c>
+      <c r="F22" s="24">
+        <v>1</v>
+      </c>
+      <c r="G22" s="24">
+        <v>1</v>
+      </c>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="25"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="57" t="s">
+      <c r="A23" s="77"/>
+      <c r="B23" s="92"/>
+      <c r="C23" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27">
-        <v>1</v>
-      </c>
-      <c r="J23" s="28"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24">
+        <v>1</v>
+      </c>
+      <c r="J23" s="25"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="B24" s="47">
+      <c r="A24" s="77"/>
+      <c r="B24" s="88">
         <v>8</v>
       </c>
-      <c r="C24" s="58" t="s">
+      <c r="C24" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27">
-        <v>1</v>
-      </c>
-      <c r="J24" s="28"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24">
+        <v>1</v>
+      </c>
+      <c r="J24" s="25"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
-      <c r="B25" s="45"/>
-      <c r="C25" s="56" t="s">
+      <c r="A25" s="77"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="26">
-        <v>1</v>
-      </c>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27">
-        <v>1</v>
-      </c>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="28">
+      <c r="D25" s="23">
+        <v>1</v>
+      </c>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24">
+        <v>1</v>
+      </c>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="57" t="s">
+      <c r="A26" s="77"/>
+      <c r="B26" s="92"/>
+      <c r="C26" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27">
-        <v>1</v>
-      </c>
-      <c r="J26" s="28"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24">
+        <v>1</v>
+      </c>
+      <c r="J26" s="25"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
-      <c r="B27" s="47">
+      <c r="A27" s="77"/>
+      <c r="B27" s="88">
         <v>9</v>
       </c>
-      <c r="C27" s="58" t="s">
+      <c r="C27" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="26">
-        <v>1</v>
-      </c>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27">
-        <v>1</v>
-      </c>
-      <c r="J27" s="28">
+      <c r="D27" s="23">
+        <v>1</v>
+      </c>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24">
+        <v>1</v>
+      </c>
+      <c r="J27" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="7"/>
-      <c r="B28" s="45"/>
-      <c r="C28" s="56" t="s">
+      <c r="A28" s="77"/>
+      <c r="B28" s="89"/>
+      <c r="C28" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="26"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="28"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
-      <c r="B29" s="46"/>
-      <c r="C29" s="57" t="s">
+      <c r="A29" s="77"/>
+      <c r="B29" s="92"/>
+      <c r="C29" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="26"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="28"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="7"/>
-      <c r="B30" s="47">
+      <c r="A30" s="77"/>
+      <c r="B30" s="88">
         <v>10</v>
       </c>
-      <c r="C30" s="58" t="s">
+      <c r="C30" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="26"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="28"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="25"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
-      <c r="B31" s="45"/>
-      <c r="C31" s="56" t="s">
+      <c r="A31" s="77"/>
+      <c r="B31" s="89"/>
+      <c r="C31" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="26">
-        <v>1</v>
-      </c>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27">
-        <v>1</v>
-      </c>
-      <c r="J31" s="28"/>
+      <c r="D31" s="23">
+        <v>1</v>
+      </c>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24">
+        <v>1</v>
+      </c>
+      <c r="J31" s="25"/>
     </row>
     <row r="32" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="59" t="s">
+      <c r="A32" s="78"/>
+      <c r="B32" s="90"/>
+      <c r="C32" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="31"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="32">
-        <v>1</v>
-      </c>
-      <c r="J32" s="33"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27">
+        <v>1</v>
+      </c>
+      <c r="J32" s="28"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="44">
-        <v>1</v>
-      </c>
-      <c r="C33" s="55" t="s">
+      <c r="B33" s="91">
+        <v>1</v>
+      </c>
+      <c r="C33" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="23">
-        <v>1</v>
-      </c>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="25">
+      <c r="D33" s="20">
+        <v>1</v>
+      </c>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="7"/>
-      <c r="B34" s="45"/>
-      <c r="C34" s="56" t="s">
+      <c r="A34" s="77"/>
+      <c r="B34" s="89"/>
+      <c r="C34" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="26"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27">
-        <v>1</v>
-      </c>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="28"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24">
+        <v>1</v>
+      </c>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="25"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="7"/>
-      <c r="B35" s="46"/>
-      <c r="C35" s="57" t="s">
+      <c r="A35" s="77"/>
+      <c r="B35" s="92"/>
+      <c r="C35" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="26"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27">
-        <v>1</v>
-      </c>
-      <c r="J35" s="28"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24">
+        <v>1</v>
+      </c>
+      <c r="J35" s="25"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="7"/>
-      <c r="B36" s="47">
+      <c r="A36" s="77"/>
+      <c r="B36" s="88">
         <v>2</v>
       </c>
-      <c r="C36" s="58" t="s">
+      <c r="C36" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="26"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="27"/>
-      <c r="J36" s="28"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="25"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="7"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="56" t="s">
+      <c r="A37" s="77"/>
+      <c r="B37" s="89"/>
+      <c r="C37" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="26">
-        <v>1</v>
-      </c>
-      <c r="E37" s="27">
-        <v>1</v>
-      </c>
-      <c r="F37" s="27">
-        <v>1</v>
-      </c>
-      <c r="G37" s="30">
-        <v>1</v>
-      </c>
-      <c r="H37" s="30">
-        <v>1</v>
-      </c>
-      <c r="I37" s="27"/>
-      <c r="J37" s="36">
+      <c r="D37" s="23">
+        <v>1</v>
+      </c>
+      <c r="E37" s="24">
+        <v>1</v>
+      </c>
+      <c r="F37" s="24">
+        <v>1</v>
+      </c>
+      <c r="G37" s="24">
+        <v>1</v>
+      </c>
+      <c r="H37" s="24">
+        <v>1</v>
+      </c>
+      <c r="I37" s="24"/>
+      <c r="J37" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="7"/>
-      <c r="B38" s="46"/>
-      <c r="C38" s="57" t="s">
+      <c r="A38" s="77"/>
+      <c r="B38" s="92"/>
+      <c r="C38" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="26"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27">
-        <v>1</v>
-      </c>
-      <c r="J38" s="28"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24">
+        <v>1</v>
+      </c>
+      <c r="J38" s="25"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="7"/>
-      <c r="B39" s="49">
+      <c r="A39" s="77"/>
+      <c r="B39" s="93">
         <v>3</v>
       </c>
-      <c r="C39" s="60" t="s">
+      <c r="C39" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="34"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="35"/>
-      <c r="H39" s="35"/>
-      <c r="I39" s="35">
-        <v>1</v>
-      </c>
-      <c r="J39" s="37"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30">
+        <v>1</v>
+      </c>
+      <c r="J39" s="31"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="7"/>
-      <c r="B40" s="50"/>
-      <c r="C40" s="56" t="s">
+      <c r="A40" s="77"/>
+      <c r="B40" s="73"/>
+      <c r="C40" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="34">
-        <v>1</v>
-      </c>
-      <c r="E40" s="35">
-        <v>1</v>
-      </c>
-      <c r="F40" s="35">
-        <v>1</v>
-      </c>
-      <c r="G40" s="35"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="35"/>
-      <c r="J40" s="37"/>
+      <c r="D40" s="29">
+        <v>1</v>
+      </c>
+      <c r="E40" s="30">
+        <v>1</v>
+      </c>
+      <c r="F40" s="30">
+        <v>1</v>
+      </c>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="31"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="7"/>
-      <c r="B41" s="51"/>
-      <c r="C41" s="61" t="s">
+      <c r="A41" s="77"/>
+      <c r="B41" s="94"/>
+      <c r="C41" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D41" s="34"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="35"/>
-      <c r="H41" s="35"/>
-      <c r="I41" s="35">
-        <v>1</v>
-      </c>
-      <c r="J41" s="37"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="30">
+        <v>1</v>
+      </c>
+      <c r="J41" s="31"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42" s="7"/>
-      <c r="B42" s="52">
+      <c r="A42" s="77"/>
+      <c r="B42" s="74">
         <v>4</v>
       </c>
-      <c r="C42" s="60" t="s">
+      <c r="C42" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="34"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="35"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="35">
-        <v>1</v>
-      </c>
-      <c r="J42" s="37"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="30">
+        <v>1</v>
+      </c>
+      <c r="J42" s="31"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" s="7"/>
-      <c r="B43" s="50"/>
-      <c r="C43" s="56" t="s">
+      <c r="A43" s="77"/>
+      <c r="B43" s="73"/>
+      <c r="C43" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="34"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35">
-        <v>1</v>
-      </c>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="37"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="30">
+        <v>1</v>
+      </c>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="31"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="7"/>
-      <c r="B44" s="51"/>
-      <c r="C44" s="61" t="s">
+      <c r="A44" s="77"/>
+      <c r="B44" s="94"/>
+      <c r="C44" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="34"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="35"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35">
-        <v>1</v>
-      </c>
-      <c r="J44" s="37"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="30">
+        <v>1</v>
+      </c>
+      <c r="J44" s="31"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="7"/>
-      <c r="B45" s="52">
+      <c r="A45" s="77"/>
+      <c r="B45" s="74">
         <v>5</v>
       </c>
-      <c r="C45" s="60" t="s">
+      <c r="C45" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D45" s="34"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="35"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="37"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="31"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" s="7"/>
-      <c r="B46" s="50"/>
-      <c r="C46" s="56" t="s">
+      <c r="A46" s="77"/>
+      <c r="B46" s="73"/>
+      <c r="C46" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D46" s="34"/>
-      <c r="E46" s="35">
-        <v>1</v>
-      </c>
-      <c r="F46" s="35"/>
-      <c r="G46" s="35">
-        <v>1</v>
-      </c>
-      <c r="H46" s="35"/>
-      <c r="I46" s="35"/>
-      <c r="J46" s="37"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="30">
+        <v>1</v>
+      </c>
+      <c r="F46" s="30"/>
+      <c r="G46" s="30">
+        <v>1</v>
+      </c>
+      <c r="H46" s="30"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
-      <c r="B47" s="53"/>
-      <c r="C47" s="62" t="s">
+      <c r="A47" s="78"/>
+      <c r="B47" s="75"/>
+      <c r="C47" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="D47" s="38"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="39"/>
-      <c r="G47" s="39"/>
-      <c r="H47" s="39"/>
-      <c r="I47" s="39">
-        <v>1</v>
-      </c>
-      <c r="J47" s="40"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="33"/>
+      <c r="I47" s="33">
+        <v>1</v>
+      </c>
+      <c r="J47" s="34"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="54">
-        <v>1</v>
-      </c>
-      <c r="C48" s="63" t="s">
+      <c r="B48" s="72">
+        <v>1</v>
+      </c>
+      <c r="C48" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="D48" s="41"/>
-      <c r="E48" s="42"/>
-      <c r="F48" s="42"/>
-      <c r="G48" s="42"/>
-      <c r="H48" s="42">
-        <v>1</v>
-      </c>
-      <c r="I48" s="42">
-        <v>1</v>
-      </c>
-      <c r="J48" s="43"/>
+      <c r="D48" s="35"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="36">
+        <v>1</v>
+      </c>
+      <c r="I48" s="36">
+        <v>1</v>
+      </c>
+      <c r="J48" s="37"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A49" s="7"/>
-      <c r="B49" s="50"/>
-      <c r="C49" s="64" t="s">
+      <c r="A49" s="77"/>
+      <c r="B49" s="73"/>
+      <c r="C49" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="34"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="35">
-        <v>1</v>
-      </c>
-      <c r="H49" s="35"/>
-      <c r="I49" s="35"/>
-      <c r="J49" s="37"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="30"/>
+      <c r="G49" s="30">
+        <v>1</v>
+      </c>
+      <c r="H49" s="30"/>
+      <c r="I49" s="30"/>
+      <c r="J49" s="31"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A50" s="7"/>
-      <c r="B50" s="52">
+      <c r="A50" s="77"/>
+      <c r="B50" s="74">
         <v>2</v>
       </c>
-      <c r="C50" s="60" t="s">
+      <c r="C50" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="D50" s="34"/>
-      <c r="E50" s="35"/>
-      <c r="F50" s="35"/>
-      <c r="G50" s="35"/>
-      <c r="H50" s="35"/>
-      <c r="I50" s="35"/>
-      <c r="J50" s="37"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="30"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="30"/>
+      <c r="J50" s="31"/>
     </row>
     <row r="51" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="8"/>
-      <c r="B51" s="53"/>
-      <c r="C51" s="62" t="s">
+      <c r="A51" s="78"/>
+      <c r="B51" s="75"/>
+      <c r="C51" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D51" s="38">
-        <v>1</v>
-      </c>
-      <c r="E51" s="39"/>
-      <c r="F51" s="39"/>
-      <c r="G51" s="39"/>
-      <c r="H51" s="39">
-        <v>1</v>
-      </c>
-      <c r="I51" s="39"/>
-      <c r="J51" s="40"/>
+      <c r="D51" s="32">
+        <v>1</v>
+      </c>
+      <c r="E51" s="33"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="33"/>
+      <c r="H51" s="33">
+        <v>1</v>
+      </c>
+      <c r="I51" s="33"/>
+      <c r="J51" s="34"/>
     </row>
     <row r="53" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="65" t="s">
+      <c r="C54" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="D54" s="12">
+      <c r="D54" s="9">
         <v>0</v>
       </c>
-      <c r="E54" s="93">
-        <v>1</v>
-      </c>
-      <c r="F54" s="13">
+      <c r="E54" s="63">
+        <v>1</v>
+      </c>
+      <c r="F54" s="10">
         <v>2</v>
       </c>
-      <c r="G54" s="93">
+      <c r="G54" s="63">
         <v>3</v>
       </c>
-      <c r="H54" s="93" t="s">
+      <c r="H54" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="I54" s="13">
+      <c r="I54" s="10">
         <v>4</v>
       </c>
-      <c r="J54" s="14" t="s">
+      <c r="J54" s="11" t="s">
         <v>4</v>
       </c>
       <c r="L54" t="s">
@@ -2390,137 +2381,137 @@
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C55" s="15" t="s">
+      <c r="C55" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D55" s="85">
+      <c r="D55" s="55">
         <f>SUM(D3,D6,D9,D12,D15,D18,D21,D24,D27,D30,D33,D36,D39,D42,D45)</f>
         <v>3</v>
       </c>
-      <c r="E55" s="16">
+      <c r="E55" s="13">
         <f t="shared" ref="E55:J55" si="0">SUM(E3,E6,E9,E12,E15,E18,E21,E24,E27,E30,E33,E36,E39,E42,E45)</f>
         <v>0</v>
       </c>
-      <c r="F55" s="16">
+      <c r="F55" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G55" s="16">
+      <c r="G55" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H55" s="16">
+      <c r="H55" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I55" s="86">
+      <c r="I55" s="56">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="J55" s="87">
+      <c r="J55" s="57">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="L55" s="66" t="s">
+      <c r="L55" s="49" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C56" s="18" t="s">
+      <c r="C56" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D56" s="83">
+      <c r="D56" s="53">
         <f t="shared" ref="D56:J56" si="1">SUM(D4,D7,D10,D13,D16,D19,D22,D25,D28,D31,D34,D37,D40,D43,D46)</f>
         <v>9</v>
       </c>
-      <c r="E56" s="84">
+      <c r="E56" s="54">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="F56" s="84">
+      <c r="F56" s="54">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="G56" s="84">
+      <c r="G56" s="54">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="H56" s="19">
+      <c r="H56" s="16">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I56" s="83">
+      <c r="I56" s="53">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="J56" s="88">
+      <c r="J56" s="58">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="L56" s="67" t="s">
+      <c r="L56" s="50" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C57" s="89" t="s">
+      <c r="C57" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="D57" s="90">
+      <c r="D57" s="60">
         <f t="shared" ref="D57:J57" si="2">SUM(D5,D8,D11,D14,D17,D20,D23,D26,D29,D32,D35,D38,D41,D44,D47)</f>
         <v>1</v>
       </c>
-      <c r="E57" s="21">
+      <c r="E57" s="18">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F57" s="90">
+      <c r="F57" s="60">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G57" s="21">
+      <c r="G57" s="18">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H57" s="21">
+      <c r="H57" s="18">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I57" s="91">
+      <c r="I57" s="61">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="J57" s="92">
+      <c r="J57" s="62">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="L57" s="68" t="s">
+      <c r="L57" s="51" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="59" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C59" s="98" t="s">
+      <c r="C59" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="D59" s="94">
+      <c r="D59" s="9">
         <v>0</v>
       </c>
-      <c r="E59" s="93">
-        <v>1</v>
-      </c>
-      <c r="F59" s="93">
+      <c r="E59" s="63">
+        <v>1</v>
+      </c>
+      <c r="F59" s="63">
         <v>2</v>
       </c>
-      <c r="G59" s="95">
+      <c r="G59" s="10">
         <v>3</v>
       </c>
-      <c r="H59" s="96" t="s">
+      <c r="H59" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="I59" s="95">
+      <c r="I59" s="10">
         <v>4</v>
       </c>
-      <c r="J59" s="97" t="s">
+      <c r="J59" s="65" t="s">
         <v>4</v>
       </c>
       <c r="L59" t="s">
@@ -2528,70 +2519,70 @@
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C60" s="15" t="s">
+      <c r="C60" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D60" s="16">
+      <c r="D60" s="13">
         <f>D48+D50</f>
         <v>0</v>
       </c>
-      <c r="E60" s="16">
+      <c r="E60" s="13">
         <f t="shared" ref="E60:J60" si="3">E48+E50</f>
         <v>0</v>
       </c>
-      <c r="F60" s="16">
+      <c r="F60" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G60" s="16">
+      <c r="G60" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H60" s="86">
+      <c r="H60" s="56">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="I60" s="86">
+      <c r="I60" s="56">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="J60" s="17">
+      <c r="J60" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L60" s="69" t="s">
+      <c r="L60" s="52" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C61" s="20" t="s">
+      <c r="C61" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D61" s="90">
+      <c r="D61" s="60">
         <f t="shared" ref="D61:J61" si="4">D49+D51</f>
         <v>1</v>
       </c>
-      <c r="E61" s="21">
+      <c r="E61" s="18">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F61" s="21">
+      <c r="F61" s="18">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G61" s="90">
+      <c r="G61" s="60">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="H61" s="90">
+      <c r="H61" s="60">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="I61" s="21">
+      <c r="I61" s="18">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J61" s="22">
+      <c r="J61" s="19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2611,18 +2602,18 @@
       <c r="L64" s="70"/>
     </row>
     <row r="65" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C65" s="99" t="s">
+      <c r="C65" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="D65" s="99"/>
-      <c r="E65" s="99"/>
-      <c r="F65" s="99"/>
-      <c r="G65" s="99"/>
-      <c r="H65" s="99"/>
-      <c r="I65" s="99"/>
-      <c r="J65" s="99"/>
-      <c r="K65" s="99"/>
-      <c r="L65" s="99"/>
+      <c r="D65" s="71"/>
+      <c r="E65" s="71"/>
+      <c r="F65" s="71"/>
+      <c r="G65" s="71"/>
+      <c r="H65" s="71"/>
+      <c r="I65" s="71"/>
+      <c r="J65" s="71"/>
+      <c r="K65" s="71"/>
+      <c r="L65" s="71"/>
     </row>
     <row r="66" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C66" s="70" t="s">
@@ -2668,22 +2659,16 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="L4:P4"/>
-    <mergeCell ref="C68:L68"/>
-    <mergeCell ref="C67:L67"/>
-    <mergeCell ref="C66:L66"/>
-    <mergeCell ref="C65:L65"/>
-    <mergeCell ref="C64:L64"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B11"/>
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="B50:B51"/>
     <mergeCell ref="A48:A51"/>
     <mergeCell ref="A3:A32"/>
     <mergeCell ref="A33:A47"/>
-    <mergeCell ref="L9:P9"/>
-    <mergeCell ref="L8:P8"/>
-    <mergeCell ref="L7:P7"/>
-    <mergeCell ref="L6:P6"/>
-    <mergeCell ref="L5:P5"/>
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="B33:B35"/>
     <mergeCell ref="B36:B38"/>
@@ -2695,12 +2680,19 @@
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="L4:P4"/>
+    <mergeCell ref="C68:L68"/>
+    <mergeCell ref="C67:L67"/>
+    <mergeCell ref="C66:L66"/>
+    <mergeCell ref="C65:L65"/>
+    <mergeCell ref="C64:L64"/>
+    <mergeCell ref="L9:P9"/>
+    <mergeCell ref="L8:P8"/>
+    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="L6:P6"/>
+    <mergeCell ref="L5:P5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>